<commit_message>
11.15-updates for the U
</commit_message>
<xml_diff>
--- a/Hours/leadership/files/leadership.xlsx
+++ b/Hours/leadership/files/leadership.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10768192\Desktop\pbischoff3.github.io\Hours\leadership\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602CEB83-ACA0-405E-A19E-2890C008BE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9D9CBF-1340-452C-AEAD-67CE7AACA7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27075" yWindow="4365" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30585" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>description</t>
   </si>
@@ -55,6 +66,9 @@
   </si>
   <si>
     <t>Station1</t>
+  </si>
+  <si>
+    <t>Stake Executive Secretary</t>
   </si>
 </sst>
 </file>
@@ -372,15 +386,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -402,13 +416,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>120</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -416,18 +430,19 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D3">
-        <v>40</v>
+        <f>C3*5</f>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -436,30 +451,51 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>112</v>
+        <f>C4*12</f>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>100</v>
       </c>
     </row>

</xml_diff>